<commit_message>
Excel text functions (LEFT, RIGHT, MID, LEN, SEARCH)
</commit_message>
<xml_diff>
--- a/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
+++ b/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\learning-excel\excel-103-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385688A5-CB05-4466-8DE0-83CDDA48FD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4680CA46-3F57-45C9-B0C8-C97E3F5ADAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="286">
   <si>
     <t>Monthly Goal:</t>
   </si>
@@ -969,6 +969,12 @@
   </si>
   <si>
     <t>EMP ID</t>
+  </si>
+  <si>
+    <t>SupplierLen</t>
+  </si>
+  <si>
+    <t>CodeLen</t>
   </si>
 </sst>
 </file>
@@ -984,7 +990,7 @@
     <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="170" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="173" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1662,7 +1668,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1979,6 +1985,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="33" xfId="11"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="33" xfId="11" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1997,25 +2010,19 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="33" xfId="11"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="33" xfId="11" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Check Cell" xfId="11" builtinId="23"/>
@@ -2729,14 +2736,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="130" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2933,13 +2940,13 @@
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="129"/>
       <c r="F12" s="3">
         <f>COUNTIF(H5:H9,"YES")</f>
         <v>3</v>
@@ -2960,10 +2967,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2976,9 +2983,10 @@
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="35" t="s">
         <v>168</v>
       </c>
@@ -3001,8 +3009,14 @@
       <c r="H2" s="36" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="22" t="s">
         <v>169</v>
       </c>
@@ -3022,11 +3036,21 @@
         <v>110</v>
       </c>
       <c r="G3" s="17" t="str">
-        <f>RIGHT(A3,2)</f>
+        <f>RIGHT(A3,LEN(A3) - 6)</f>
         <v>WW</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="11">
+        <f>LEN(A3)</f>
+        <v>8</v>
+      </c>
+      <c r="I3" s="11">
+        <v>3</v>
+      </c>
+      <c r="J3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="22" t="s">
         <v>170</v>
       </c>
@@ -3037,11 +3061,24 @@
         <v>12.19</v>
       </c>
       <c r="D4" s="37"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="E4" s="17" t="str">
+        <f t="shared" ref="E4:E26" si="0">LEFT(A4,3)</f>
+        <v>ACM</v>
+      </c>
+      <c r="F4" s="17" t="str">
+        <f t="shared" ref="F4:F26" si="1">MID(A4,4,3)</f>
+        <v>111</v>
+      </c>
+      <c r="G4" s="17" t="str">
+        <f t="shared" ref="G4:G26" si="2">RIGHT(A4,LEN(A4) - 6)</f>
+        <v>WW</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" ref="H4:H26" si="3">LEN(A4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="22" t="s">
         <v>171</v>
       </c>
@@ -3052,11 +3089,24 @@
         <v>10.89</v>
       </c>
       <c r="D5" s="37"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="E5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="G5" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>WW</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="22" t="s">
         <v>172</v>
       </c>
@@ -3067,11 +3117,24 @@
         <v>9.75</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="E6" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F6" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="G6" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="22" t="s">
         <v>173</v>
       </c>
@@ -3082,11 +3145,24 @@
         <v>9.59</v>
       </c>
       <c r="D7" s="37"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="E7" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F7" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>322</v>
+      </c>
+      <c r="G7" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="22" t="s">
         <v>174</v>
       </c>
@@ -3097,11 +3173,24 @@
         <v>10.4</v>
       </c>
       <c r="D8" s="37"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="E8" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F8" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>325</v>
+      </c>
+      <c r="G8" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="22" t="s">
         <v>175</v>
       </c>
@@ -3112,11 +3201,24 @@
         <v>10.56</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="E9" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="G9" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="22" t="s">
         <v>176</v>
       </c>
@@ -3127,11 +3229,24 @@
         <v>9.75</v>
       </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E10" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="G10" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="22" t="s">
         <v>177</v>
       </c>
@@ -3142,11 +3257,24 @@
         <v>9.75</v>
       </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="E11" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>ACM</v>
+      </c>
+      <c r="F11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="G11" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>DP</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="22" t="s">
         <v>204</v>
       </c>
@@ -3157,11 +3285,24 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="E12" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F12" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>530</v>
+      </c>
+      <c r="G12" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OL</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="22" t="s">
         <v>205</v>
       </c>
@@ -3172,11 +3313,24 @@
         <v>5.04</v>
       </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="E13" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F13" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>TF</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="22" t="s">
         <v>206</v>
       </c>
@@ -3187,11 +3341,24 @@
         <v>3.9</v>
       </c>
       <c r="D14" s="37"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="E14" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F14" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="G14" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OL</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="22" t="s">
         <v>207</v>
       </c>
@@ -3202,11 +3369,24 @@
         <v>4.55</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="E15" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F15" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="G15" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OL</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="22" t="s">
         <v>208</v>
       </c>
@@ -3217,11 +3397,24 @@
         <v>5.2</v>
       </c>
       <c r="D16" s="37"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="E16" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F16" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="G16" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>GO</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="22" t="s">
         <v>209</v>
       </c>
@@ -3232,11 +3425,24 @@
         <v>7.31</v>
       </c>
       <c r="D17" s="37"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="E17" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="G17" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>BF</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="22" t="s">
         <v>210</v>
       </c>
@@ -3247,11 +3453,24 @@
         <v>6.5</v>
       </c>
       <c r="D18" s="37"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="E18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="G18" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>PS</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="22" t="s">
         <v>178</v>
       </c>
@@ -3262,11 +3481,24 @@
         <v>4.55</v>
       </c>
       <c r="D19" s="37"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="E19" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AST</v>
+      </c>
+      <c r="F19" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="G19" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>0995</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="22" t="s">
         <v>211</v>
       </c>
@@ -3277,11 +3509,24 @@
         <v>14.3</v>
       </c>
       <c r="D20" s="37"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="E20" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>BVR</v>
+      </c>
+      <c r="F20" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>590</v>
+      </c>
+      <c r="G20" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>WF</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="22" t="s">
         <v>212</v>
       </c>
@@ -3292,11 +3537,24 @@
         <v>13.81</v>
       </c>
       <c r="D21" s="37"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="E21" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>BVR</v>
+      </c>
+      <c r="F21" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>690</v>
+      </c>
+      <c r="G21" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AF</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="22" t="s">
         <v>217</v>
       </c>
@@ -3307,11 +3565,24 @@
         <v>7.31</v>
       </c>
       <c r="D22" s="37"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="E22" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRA</v>
+      </c>
+      <c r="F22" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+      <c r="G22" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OF</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="22" t="s">
         <v>218</v>
       </c>
@@ -3322,11 +3593,24 @@
         <v>7.31</v>
       </c>
       <c r="D23" s="37"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="E23" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRA</v>
+      </c>
+      <c r="F23" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="G23" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OF</v>
+      </c>
+      <c r="H23" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="22" t="s">
         <v>214</v>
       </c>
@@ -3337,11 +3621,24 @@
         <v>7.31</v>
       </c>
       <c r="D24" s="37"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="E24" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRA</v>
+      </c>
+      <c r="F24" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="G24" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OF</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="22" t="s">
         <v>215</v>
       </c>
@@ -3352,11 +3649,24 @@
         <v>7.64</v>
       </c>
       <c r="D25" s="37"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="E25" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRA</v>
+      </c>
+      <c r="F25" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="G25" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OF</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="22" t="s">
         <v>216</v>
       </c>
@@ -3367,9 +3677,22 @@
         <v>6.14</v>
       </c>
       <c r="D26" s="37"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="E26" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRA</v>
+      </c>
+      <c r="F26" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>610</v>
+      </c>
+      <c r="G26" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>OF</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3384,7 +3707,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3406,28 +3729,68 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="137" t="s">
         <v>243</v>
       </c>
+      <c r="B2" s="11" t="str">
+        <f>LEFT(A2,SEARCH(" ",A2))</f>
+        <v xml:space="preserve">Patrick </v>
+      </c>
+      <c r="C2" s="11" t="str">
+        <f>RIGHT(A2,LEN(A2)-SEARCH(" ",A2))</f>
+        <v>Marleau</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="137" t="s">
         <v>244</v>
       </c>
+      <c r="B3" s="11" t="str">
+        <f t="shared" ref="B3:B6" si="0">LEFT(A3,SEARCH(" ",A3))</f>
+        <v xml:space="preserve">Joe </v>
+      </c>
+      <c r="C3" s="11" t="str">
+        <f t="shared" ref="C3:C6" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
+        <v>Thornton</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="137" t="s">
         <v>245</v>
       </c>
+      <c r="B4" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Brent </v>
+      </c>
+      <c r="C4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Burns</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="137" t="s">
         <v>246</v>
       </c>
+      <c r="B5" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Joe </v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavelski</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="137" t="s">
         <v>247</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Martin </v>
+      </c>
+      <c r="C6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Jones</v>
       </c>
     </row>
   </sheetData>
@@ -3441,8 +3804,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3460,10 +3823,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="133" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="133"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="25" t="s">
@@ -3472,11 +3835,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="134" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="135"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="25" t="s">
@@ -3485,8 +3848,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="134" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,C4,B4)</f>
+        <v>Joe Gonzales</v>
+      </c>
+      <c r="F4" s="135"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="25" t="s">
@@ -3495,8 +3861,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="134" t="str">
+        <f>_xlfn.CONCAT(C5," ",B5)</f>
+        <v>Gail Scote</v>
+      </c>
+      <c r="F5" s="135"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="25" t="s">
@@ -3505,8 +3874,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="134" t="str">
+        <f t="shared" ref="E6:E18" si="0">_xlfn.CONCAT(C6," ",B6)</f>
+        <v>Sheryl Kane</v>
+      </c>
+      <c r="F6" s="135"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="25" t="s">
@@ -3515,8 +3887,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Kendrick Hapsbuch</v>
+      </c>
+      <c r="F7" s="135"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="25" t="s">
@@ -3525,8 +3900,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Henders</v>
+      </c>
+      <c r="F8" s="135"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="25" t="s">
@@ -3535,8 +3913,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Katie Atherton</v>
+      </c>
+      <c r="F9" s="135"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="25" t="s">
@@ -3545,8 +3926,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Frank Bellwood</v>
+      </c>
+      <c r="F10" s="135"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="25" t="s">
@@ -3555,8 +3939,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Linda Cooper</v>
+      </c>
+      <c r="F11" s="135"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="25" t="s">
@@ -3565,8 +3952,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Brent Cronwith</v>
+      </c>
+      <c r="F12" s="135"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="25" t="s">
@@ -3575,8 +3965,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Sandrae Simpson</v>
+      </c>
+      <c r="F13" s="135"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="25" t="s">
@@ -3585,8 +3978,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Randy Sindole</v>
+      </c>
+      <c r="F14" s="135"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="25" t="s">
@@ -3595,8 +3991,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Ellen Smith</v>
+      </c>
+      <c r="F15" s="135"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="25" t="s">
@@ -3605,8 +4004,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuome Vuanuo</v>
+      </c>
+      <c r="F16" s="135"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="25" t="s">
@@ -3615,8 +4017,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Tadeuz Szcznyck</v>
+      </c>
+      <c r="F17" s="135"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="25" t="s">
@@ -3625,11 +4030,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="134" t="str">
+        <f t="shared" si="0"/>
+        <v>Tammy Wu</v>
+      </c>
+      <c r="F18" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3640,13 +4055,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3678,14 +4086,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3904,13 +4312,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="129"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -3980,14 +4388,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="130" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -4207,13 +4615,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="129"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -4759,10 +5167,10 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="136" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="133"/>
+      <c r="C10" s="136"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="113" t="s">
@@ -13853,7 +14261,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -13871,10 +14279,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="131" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="132"/>
     </row>
     <row r="3" spans="1:5" ht="17.25" thickTop="1" thickBot="1">
       <c r="A3" s="61" t="s">
@@ -14210,10 +14618,10 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B10" s="134"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="134"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="124"/>
       <c r="F10" s="32" t="s">
         <v>21</v>
       </c>
@@ -14285,10 +14693,10 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B17" s="134"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="134"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="124"/>
       <c r="F17" s="32" t="s">
         <v>23</v>
       </c>
@@ -14299,7 +14707,7 @@
       </c>
       <c r="C18" s="68"/>
       <c r="D18" s="68"/>
-      <c r="F18" s="136">
+      <c r="F18" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B18,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>33344</v>
       </c>
@@ -14310,7 +14718,7 @@
       </c>
       <c r="C19" s="68"/>
       <c r="D19" s="68"/>
-      <c r="F19" s="136">
+      <c r="F19" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B19,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>31503</v>
       </c>
@@ -14321,7 +14729,7 @@
       </c>
       <c r="C20" s="68"/>
       <c r="D20" s="68"/>
-      <c r="F20" s="136">
+      <c r="F20" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B20,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>31051</v>
       </c>
@@ -14332,7 +14740,7 @@
       </c>
       <c r="C21" s="68"/>
       <c r="D21" s="68"/>
-      <c r="F21" s="136">
+      <c r="F21" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B21,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>32863</v>
       </c>
@@ -14343,7 +14751,7 @@
       </c>
       <c r="C22" s="68"/>
       <c r="D22" s="68"/>
-      <c r="F22" s="136">
+      <c r="F22" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B22,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>32561</v>
       </c>
@@ -14354,16 +14762,16 @@
       </c>
       <c r="C23" s="68"/>
       <c r="D23" s="68"/>
-      <c r="F23" s="136">
+      <c r="F23" s="126">
         <f>INDEX('INDEX MATCH Master Emp List'!$H$1:$H$38,MATCH(B23,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>31217</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B24" s="134"/>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="134"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="32" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Complete Excel 365 functions module: FILTER/SORT/UNIQUE, XLOOKUP, SWITCH(TRUE), TEXTJOIN, TEXTSPLIT
</commit_message>
<xml_diff>
--- a/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
+++ b/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\learning-excel\excel-103-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4680CA46-3F57-45C9-B0C8-C97E3F5ADAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E44F223-ADA7-4420-9160-CC3311FA859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1992,6 +1992,7 @@
     <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -2010,19 +2011,18 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Check Cell" xfId="11" builtinId="23"/>
@@ -2736,14 +2736,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2940,13 +2940,13 @@
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="127" t="s">
+      <c r="A12" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="129"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="3">
         <f>COUNTIF(H5:H9,"YES")</f>
         <v>3</v>
@@ -2969,8 +2969,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3706,8 +3706,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3729,7 +3729,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="127" t="s">
         <v>243</v>
       </c>
       <c r="B2" s="11" t="str">
@@ -3742,7 +3742,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="127" t="s">
         <v>244</v>
       </c>
       <c r="B3" s="11" t="str">
@@ -3755,7 +3755,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="127" t="s">
         <v>245</v>
       </c>
       <c r="B4" s="11" t="str">
@@ -3768,7 +3768,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="127" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="11" t="str">
@@ -3781,7 +3781,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="137" t="s">
+      <c r="A6" s="127" t="s">
         <v>247</v>
       </c>
       <c r="B6" s="11" t="str">
@@ -3789,7 +3789,7 @@
         <v xml:space="preserve">Martin </v>
       </c>
       <c r="C6" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.TEXTAFTER(A6," ",-1,0,0)</f>
         <v>Jones</v>
       </c>
     </row>
@@ -3804,8 +3804,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3823,10 +3823,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="133" t="s">
+      <c r="E2" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="133"/>
+      <c r="F2" s="136"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="25" t="s">
@@ -4038,13 +4038,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -4055,6 +4048,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4086,14 +4086,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -4312,13 +4312,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="127" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="128"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="129"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -4388,14 +4388,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -4615,13 +4615,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="127" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="128"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="129"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -5167,10 +5167,10 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="137" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="136"/>
+      <c r="C10" s="137"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="113" t="s">
@@ -12749,7 +12749,7 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F3" sqref="F3:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12790,15 +12790,15 @@
         <v>howards</v>
       </c>
       <c r="D3" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B3,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>148</v>
       </c>
       <c r="E3" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B3,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>11.25</v>
       </c>
       <c r="F3" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B3,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AT</v>
       </c>
       <c r="G3" s="67"/>
@@ -12812,15 +12812,15 @@
         <v>joeg</v>
       </c>
       <c r="D4" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B4,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>121</v>
       </c>
       <c r="E4" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B4,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>12.25</v>
       </c>
       <c r="F4" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B4,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AT</v>
       </c>
       <c r="G4" s="67"/>
@@ -12834,15 +12834,15 @@
         <v>gails</v>
       </c>
       <c r="D5" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B5,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>123</v>
       </c>
       <c r="E5" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B5,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>14.55</v>
       </c>
       <c r="F5" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B5,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AT</v>
       </c>
       <c r="G5" s="67"/>
@@ -12856,15 +12856,15 @@
         <v>sherylk</v>
       </c>
       <c r="D6" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B6,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>126</v>
       </c>
       <c r="E6" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B6,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>11.25</v>
       </c>
       <c r="F6" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B6,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AD</v>
       </c>
       <c r="G6" s="67"/>
@@ -12878,15 +12878,15 @@
         <v>kendrickh</v>
       </c>
       <c r="D7" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B7,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>101</v>
       </c>
       <c r="E7" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B7,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>10.199999999999999</v>
       </c>
       <c r="F7" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B7,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AC</v>
       </c>
       <c r="G7" s="67"/>
@@ -12900,15 +12900,15 @@
         <v>markh</v>
       </c>
       <c r="D8" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B8,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>118</v>
       </c>
       <c r="E8" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B8,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>12.25</v>
       </c>
       <c r="F8" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B8,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AD</v>
       </c>
       <c r="G8" s="67"/>
@@ -12922,15 +12922,15 @@
         <v>katiea</v>
       </c>
       <c r="D9" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B9,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>289</v>
       </c>
       <c r="E9" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B9,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>9.9499999999999993</v>
       </c>
       <c r="F9" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B9,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>HR</v>
       </c>
       <c r="G9" s="67"/>
@@ -12944,15 +12944,15 @@
         <v>frankb</v>
       </c>
       <c r="D10" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B10,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>124</v>
       </c>
       <c r="E10" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B10,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>12.3</v>
       </c>
       <c r="F10" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B10,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>MK</v>
       </c>
       <c r="G10" s="67"/>
@@ -12964,15 +12964,15 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B11,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E11" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B11,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F11" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B11,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G11" s="67"/>
@@ -12984,15 +12984,15 @@
         <v>#N/A</v>
       </c>
       <c r="D12" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B12,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E12" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B12,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F12" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B12,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G12" s="67"/>
@@ -13004,15 +13004,15 @@
         <v>#N/A</v>
       </c>
       <c r="D13" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B13,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E13" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B13,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F13" s="11" t="e">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B13,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G13" s="67"/>
@@ -13026,15 +13026,15 @@
         <v>randys</v>
       </c>
       <c r="D14" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B14,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>139</v>
       </c>
       <c r="E14" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B14,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>14.25</v>
       </c>
       <c r="F14" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B14,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>MK</v>
       </c>
       <c r="G14" s="67"/>
@@ -13048,15 +13048,15 @@
         <v>ellens</v>
       </c>
       <c r="D15" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B15,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>137</v>
       </c>
       <c r="E15" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B15,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>11.5</v>
       </c>
       <c r="F15" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B15,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>MF</v>
       </c>
       <c r="G15" s="67"/>
@@ -13070,15 +13070,15 @@
         <v>tuomev</v>
       </c>
       <c r="D16" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B16,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>151</v>
       </c>
       <c r="E16" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B16,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>10.35</v>
       </c>
       <c r="F16" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B16,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AC</v>
       </c>
       <c r="G16" s="67"/>
@@ -13092,15 +13092,15 @@
         <v>tadeuzs</v>
       </c>
       <c r="D17" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B17,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>122</v>
       </c>
       <c r="E17" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B17,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>10.15</v>
       </c>
       <c r="F17" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B17,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>HR</v>
       </c>
       <c r="G17" s="67"/>
@@ -13114,15 +13114,15 @@
         <v>tammyw</v>
       </c>
       <c r="D18" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B18,'Master Emp List'!$A$1:$I$38,6,FALSE)</f>
         <v>132</v>
       </c>
       <c r="E18" s="11">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B18,'Master Emp List'!$A$1:$I$38,9,FALSE)</f>
         <v>12.25</v>
       </c>
       <c r="F18" s="11" t="str">
-        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <f>VLOOKUP(B18,'Master Emp List'!$A$1:$I$38,4,FALSE)</f>
         <v>AD</v>
       </c>
       <c r="G18" s="67"/>
@@ -13138,7 +13138,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
@@ -14262,7 +14262,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14279,10 +14279,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" thickBot="1"/>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="132" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="133"/>
     </row>
     <row r="3" spans="1:5" ht="17.25" thickTop="1" thickBot="1">
       <c r="A3" s="61" t="s">
@@ -14383,7 +14383,7 @@
   <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14494,8 +14494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14783,7 +14783,7 @@
       <c r="C25" s="68"/>
       <c r="D25" s="68"/>
       <c r="F25" s="68" t="str">
-        <f>VLOOKUP($B25,'INDEX MATCH Master Emp List'!A1:I38,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B25,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 1</v>
       </c>
     </row>
@@ -14794,7 +14794,7 @@
       <c r="C26" s="68"/>
       <c r="D26" s="68"/>
       <c r="F26" s="68" t="str">
-        <f>VLOOKUP($B26,'INDEX MATCH Master Emp List'!A2:I39,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B26,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 2</v>
       </c>
     </row>
@@ -14805,7 +14805,7 @@
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
       <c r="F27" s="68" t="str">
-        <f>VLOOKUP($B27,'INDEX MATCH Master Emp List'!A3:I40,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B27,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 1</v>
       </c>
     </row>
@@ -14816,7 +14816,7 @@
       <c r="C28" s="68"/>
       <c r="D28" s="68"/>
       <c r="F28" s="68" t="str">
-        <f>VLOOKUP($B28,'INDEX MATCH Master Emp List'!A4:I41,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B28,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 1</v>
       </c>
     </row>
@@ -14827,7 +14827,7 @@
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
       <c r="F29" s="68" t="str">
-        <f>VLOOKUP($B29,'INDEX MATCH Master Emp List'!A5:I42,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B29,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 2</v>
       </c>
     </row>
@@ -14838,7 +14838,7 @@
       <c r="C30" s="68"/>
       <c r="D30" s="68"/>
       <c r="F30" s="68" t="str">
-        <f>VLOOKUP($B30,'INDEX MATCH Master Emp List'!A6:I43,MATCH("Location",'INDEX MATCH Master Emp List'!$A$1:$I$1,0),FALSE)</f>
+        <f>INDEX('INDEX MATCH Master Emp List'!$G$1:$G$38,MATCH(B30,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
         <v>Building 1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Excel practice notes and exercises: auditing, worksheet protection, what-if tools, macros
</commit_message>
<xml_diff>
--- a/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
+++ b/learning-excel/excel-103-course/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\learning-excel\excel-103-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E44F223-ADA7-4420-9160-CC3311FA859E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CEF991-7395-4FDF-AF30-A013E3B7ED6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -110,6 +110,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2011,13 +2014,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3706,7 +3709,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3750,7 +3753,7 @@
         <v xml:space="preserve">Joe </v>
       </c>
       <c r="C3" s="11" t="str">
-        <f t="shared" ref="C3:C6" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
+        <f t="shared" ref="C3:C5" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
         <v>Thornton</v>
       </c>
     </row>
@@ -3823,10 +3826,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="136" t="s">
+      <c r="E2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="136"/>
+      <c r="F2" s="134"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="25" t="s">
@@ -3835,11 +3838,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="134" t="str">
+      <c r="E3" s="135" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="135"/>
+      <c r="F3" s="136"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="25" t="s">
@@ -3848,11 +3851,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="134" t="str">
+      <c r="E4" s="135" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,C4,B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="135"/>
+      <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="25" t="s">
@@ -3861,11 +3864,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="134" t="str">
+      <c r="E5" s="135" t="str">
         <f>_xlfn.CONCAT(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="135"/>
+      <c r="F5" s="136"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="25" t="s">
@@ -3874,11 +3877,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="134" t="str">
+      <c r="E6" s="135" t="str">
         <f t="shared" ref="E6:E18" si="0">_xlfn.CONCAT(C6," ",B6)</f>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="135"/>
+      <c r="F6" s="136"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="25" t="s">
@@ -3887,11 +3890,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="134" t="str">
+      <c r="E7" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="135"/>
+      <c r="F7" s="136"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="25" t="s">
@@ -3900,11 +3903,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="134" t="str">
+      <c r="E8" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="135"/>
+      <c r="F8" s="136"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="25" t="s">
@@ -3913,11 +3916,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="134" t="str">
+      <c r="E9" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="135"/>
+      <c r="F9" s="136"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="25" t="s">
@@ -3926,11 +3929,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="134" t="str">
+      <c r="E10" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="135"/>
+      <c r="F10" s="136"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="25" t="s">
@@ -3939,11 +3942,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="134" t="str">
+      <c r="E11" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="135"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="25" t="s">
@@ -3952,11 +3955,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="134" t="str">
+      <c r="E12" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="135"/>
+      <c r="F12" s="136"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="25" t="s">
@@ -3965,11 +3968,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="134" t="str">
+      <c r="E13" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="135"/>
+      <c r="F13" s="136"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="25" t="s">
@@ -3978,11 +3981,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="134" t="str">
+      <c r="E14" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="135"/>
+      <c r="F14" s="136"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="25" t="s">
@@ -3991,11 +3994,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="134" t="str">
+      <c r="E15" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="135"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="25" t="s">
@@ -4004,11 +4007,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="134" t="str">
+      <c r="E16" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="135"/>
+      <c r="F16" s="136"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="25" t="s">
@@ -4017,11 +4020,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="134" t="str">
+      <c r="E17" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="135"/>
+      <c r="F17" s="136"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="25" t="s">
@@ -4030,14 +4033,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="134" t="str">
+      <c r="E18" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="135"/>
+      <c r="F18" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -4048,13 +4058,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4068,7 +4071,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4361,6 +4364,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cellWatches>
+    <cellWatch r="B2"/>
+  </cellWatches>
 </worksheet>
 </file>
 
@@ -4369,8 +4375,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4628,6 +4634,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="niHvW8jr3BPVLq+5wrcpgRVoDflEeDcXji82RaKmlNr/7kHQODRSBwQ0NHJcS38uJHhxy7nhJXVbB7GRsoMWYw==" saltValue="hVpP5EmfTYwGtOZepge3sA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A14:E14"/>

</xml_diff>